<commit_message>
add box and change time process
add box and change time process
</commit_message>
<xml_diff>
--- a/Excel2Lua/bin/Debug/excel/七天乐.xlsx
+++ b/Excel2Lua/bin/Debug/excel/七天乐.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="1"/>
@@ -10,7 +10,7 @@
     <sheet name="通用" sheetId="1" r:id="rId1"/>
     <sheet name="七天乐" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -601,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -777,7 +777,7 @@
         <v>1</v>
       </c>
       <c r="O3" s="9">
-        <v>1296000</v>
+        <v>15</v>
       </c>
       <c r="P3" s="10">
         <v>937</v>
@@ -787,7 +787,7 @@
         <v>1</v>
       </c>
       <c r="S3" s="9">
-        <v>1296000</v>
+        <v>15</v>
       </c>
       <c r="T3" s="11"/>
       <c r="U3" s="7">
@@ -1282,7 +1282,7 @@
         <v>1</v>
       </c>
       <c r="O12" s="9">
-        <v>1296000</v>
+        <v>15</v>
       </c>
       <c r="P12" s="10">
         <v>9050</v>
@@ -1292,7 +1292,7 @@
         <v>1</v>
       </c>
       <c r="S12" s="9">
-        <v>1296000</v>
+        <v>15</v>
       </c>
       <c r="T12" s="11"/>
       <c r="U12" s="7">

</xml_diff>